<commit_message>
Revert "added version 5"
This reverts commit c5099fa66da959585316a18c96be5e15e8df4ff8.
</commit_message>
<xml_diff>
--- a/myexcel.xlsx
+++ b/myexcel.xlsx
@@ -16,15 +16,12 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3" uniqueCount="3">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2" uniqueCount="2">
   <si>
     <t>assim</t>
   </si>
   <si>
     <t>ujjwal</t>
-  </si>
-  <si>
-    <t>how are you</t>
   </si>
 </sst>
 </file>
@@ -356,23 +353,20 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:D1"/>
+  <dimension ref="A1:B1"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D1" sqref="D1"/>
+      <selection activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:4">
+    <row r="1" spans="1:2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
       <c r="B1" t="s">
         <v>1</v>
-      </c>
-      <c r="D1" t="s">
-        <v>2</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Revert "Revert "added version 5""
This reverts commit 52ed9e809120770bb06ae93dc377efd3d52a9df7.
</commit_message>
<xml_diff>
--- a/myexcel.xlsx
+++ b/myexcel.xlsx
@@ -16,12 +16,15 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2" uniqueCount="2">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3" uniqueCount="3">
   <si>
     <t>assim</t>
   </si>
   <si>
     <t>ujjwal</t>
+  </si>
+  <si>
+    <t>how are you</t>
   </si>
 </sst>
 </file>
@@ -353,20 +356,23 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:B1"/>
+  <dimension ref="A1:D1"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B1" sqref="B1"/>
+      <selection activeCell="D1" sqref="D1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:2">
+    <row r="1" spans="1:4">
       <c r="A1" t="s">
         <v>0</v>
       </c>
       <c r="B1" t="s">
         <v>1</v>
+      </c>
+      <c r="D1" t="s">
+        <v>2</v>
       </c>
     </row>
   </sheetData>

</xml_diff>